<commit_message>
Found quantity errors on BOM after last check in for Rev changes.  Also added transparent background pics of 3D PCB assembly render.
</commit_message>
<xml_diff>
--- a/Hardware/BOM/MSP430AFE253_Demo_Board_BOM.xlsx
+++ b/Hardware/BOM/MSP430AFE253_Demo_Board_BOM.xlsx
@@ -47,9 +47,6 @@
     <t>CAP CER 0.1UF 10V 10% X7R 0603</t>
   </si>
   <si>
-    <t>C13,C11,C10,C9,C6,C5,C1,C2</t>
-  </si>
-  <si>
     <t>0603</t>
   </si>
   <si>
@@ -131,18 +128,12 @@
     <t>RES 1M OHM 1/10W 5% 0603 SMD</t>
   </si>
   <si>
-    <t>R13,R7</t>
-  </si>
-  <si>
     <t>RMCF0603JT47K0</t>
   </si>
   <si>
     <t>RES 47K OHM 1/10W 5% 0603 SMD</t>
   </si>
   <si>
-    <t>R16,R3,R4,R5,R11,R15</t>
-  </si>
-  <si>
     <t>RMCF0603JT750R</t>
   </si>
   <si>
@@ -161,9 +152,6 @@
     <t>RES 0.0 OHM 1/10W 0603 SMD</t>
   </si>
   <si>
-    <t>R6,R8,R14,R12</t>
-  </si>
-  <si>
     <t>RMCF0603JT33R0</t>
   </si>
   <si>
@@ -264,6 +252,18 @@
   </si>
   <si>
     <t>RES 270 OHM 1/10W 5% 0603</t>
+  </si>
+  <si>
+    <t>C13,C11,C6,C5,C1,C2</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R3,R11</t>
+  </si>
+  <si>
+    <t>R14,R12</t>
   </si>
 </sst>
 </file>
@@ -335,7 +335,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -345,8 +344,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -655,19 +659,19 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -707,13 +711,13 @@
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="G2" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -721,19 +725,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
+      <c r="F3" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G3" s="3">
         <v>5</v>
@@ -744,19 +748,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>11</v>
+      <c r="F4" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -767,19 +771,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>11</v>
+      <c r="F5" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -790,19 +794,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>11</v>
+      <c r="F6" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -813,18 +817,18 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="3">
         <v>1</v>
       </c>
@@ -834,18 +838,18 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="3">
         <v>1</v>
       </c>
@@ -855,21 +859,21 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="13">
+      <c r="F9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="11">
         <v>2</v>
       </c>
     </row>
@@ -878,22 +882,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="13">
-        <v>2</v>
+      <c r="E10" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -901,22 +905,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="13">
-        <v>6</v>
+        <v>38</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -924,21 +928,21 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="13">
+        <v>40</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="11">
         <v>1</v>
       </c>
     </row>
@@ -947,22 +951,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G13" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -970,19 +974,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>11</v>
+        <v>46</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G14" s="3">
         <v>2</v>
@@ -993,18 +997,17 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15"/>
+        <v>50</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="G15" s="3">
         <v>3</v>
       </c>
@@ -1014,18 +1017,18 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3"/>
       <c r="G16" s="3">
         <v>1</v>
       </c>
@@ -1035,19 +1038,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="G17" s="3">
         <v>1</v>
@@ -1058,19 +1061,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="G18" s="3">
         <v>1</v>
@@ -1081,18 +1084,18 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="3"/>
       <c r="G19" s="3">
         <v>1</v>
       </c>
@@ -1102,18 +1105,18 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="3">
         <v>3</v>
       </c>
@@ -1123,18 +1126,18 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="3">
         <v>1</v>
       </c>

</xml_diff>